<commit_message>
update this is me
</commit_message>
<xml_diff>
--- a/ThisIsMe_2025.xlsx
+++ b/ThisIsMe_2025.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -1619,9 +1619,7 @@
       <c r="C18" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>7</v>
-      </c>
+      <c r="D18" s="30"/>
       <c r="E18" s="32" t="s">
         <v>40</v>
       </c>
@@ -1941,9 +1939,7 @@
       <c r="C27" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>7</v>
-      </c>
+      <c r="D27" s="30"/>
       <c r="E27" s="35"/>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>

</xml_diff>